<commit_message>
changes made to tasklist
</commit_message>
<xml_diff>
--- a/ABML_PendingTask23.xlsx
+++ b/ABML_PendingTask23.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Service DC &amp; Sales Invoice</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Venetex Reprocesing</t>
+  </si>
+  <si>
+    <t>DO Schedule Correction</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -548,8 +551,12 @@
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="4">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3">

</xml_diff>